<commit_message>
About to redo some names with spurious epochs
</commit_message>
<xml_diff>
--- a/AGN_outlier_flux_W1.xlsx
+++ b/AGN_outlier_flux_W1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ciara\Dropbox\University\University Work\Fourth Year\Project\New_project_repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41F5A75D-8F30-433E-A3A4-9C8F2E5D80B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEBACE7-CA9F-49A1-9795-529DD4E29121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25A9BF87-2C41-4EEB-99F2-D3078486E8B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>AGN</t>
   </si>
@@ -78,6 +78,27 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>122321.78+311410.6</t>
+  </si>
+  <si>
+    <t>151354.51+184804.3</t>
+  </si>
+  <si>
+    <t>124939.87+581115.5</t>
+  </si>
+  <si>
+    <t>155021.33+432712.6</t>
+  </si>
+  <si>
+    <t>111353.73+515725.8</t>
+  </si>
+  <si>
+    <t>162659.42+424450.0</t>
   </si>
 </sst>
 </file>
@@ -458,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98A105A-AECB-4A17-87C6-F1F8EE52DB15}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,18 +540,18 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -547,62 +568,186 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12">
         <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some things. Nice and tidy now!
</commit_message>
<xml_diff>
--- a/AGN_outlier_flux_W1.xlsx
+++ b/AGN_outlier_flux_W1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ciara\Dropbox\University\University Work\Fourth Year\Project\New_project_repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5429A508-71C7-4E09-BCDA-2F8B36BDE509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741F3CF7-290A-45E3-A773-A3A1B7A7C8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9C39F9C0-EC1E-45A7-A869-AAB69C3080A6}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Did lots. Created plots. remove_outliers function also
</commit_message>
<xml_diff>
--- a/AGN_outlier_flux_W1.xlsx
+++ b/AGN_outlier_flux_W1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ciara\Dropbox\University\University Work\Fourth Year\Project\New_project_repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741F3CF7-290A-45E3-A773-A3A1B7A7C8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81741950-9FE3-4A3E-9952-E2FD5EBB06AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9C39F9C0-EC1E-45A7-A869-AAB69C3080A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>AGN</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Sample 2</t>
-  </si>
-  <si>
-    <t>162003.10+552822.4</t>
   </si>
   <si>
     <t>Sample 3</t>
@@ -452,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA315B97-A88E-4567-8390-A61EB3B13A00}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,24 +503,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>